<commit_message>
Convert 3SKJ heavy chain data to Kabat numbering.
</commit_message>
<xml_diff>
--- a/experimental_data/experimental_data.xlsx
+++ b/experimental_data/experimental_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="177">
   <si>
     <t>pdbid</t>
   </si>
@@ -291,25 +291,25 @@
     <t>H-G52R</t>
   </si>
   <si>
-    <t>H-A107I</t>
-  </si>
-  <si>
-    <t>H-V108M</t>
-  </si>
-  <si>
-    <t>H-A109F</t>
-  </si>
-  <si>
-    <t>H-A109I</t>
-  </si>
-  <si>
-    <t>H-A109K</t>
-  </si>
-  <si>
-    <t>H-A109M</t>
-  </si>
-  <si>
-    <t>H-P111Y</t>
+    <t>H-A100CI</t>
+  </si>
+  <si>
+    <t>H-V100DM</t>
+  </si>
+  <si>
+    <t>H-A100EF</t>
+  </si>
+  <si>
+    <t>H-A100EI</t>
+  </si>
+  <si>
+    <t>H-A100EK</t>
+  </si>
+  <si>
+    <t>H-A100EM</t>
+  </si>
+  <si>
+    <t>H-P100GY</t>
   </si>
   <si>
     <t>L-S30W</t>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>IL13</t>
+  </si>
+  <si>
+    <t>pM</t>
   </si>
   <si>
     <t>Supplemental Table 2</t>
@@ -2956,7 +2959,7 @@
       <c r="E4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>89</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -2974,7 +2977,7 @@
       <c r="K4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
@@ -2992,7 +2995,7 @@
       <c r="E5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>90</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -3010,7 +3013,7 @@
       <c r="K5" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
@@ -3028,7 +3031,7 @@
       <c r="E6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>91</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -3046,7 +3049,7 @@
       <c r="K6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
@@ -3064,7 +3067,7 @@
       <c r="E7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -3082,7 +3085,7 @@
       <c r="K7" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
@@ -3100,7 +3103,7 @@
       <c r="E8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>93</v>
       </c>
       <c r="G8" s="5" t="s">
@@ -3118,7 +3121,7 @@
       <c r="K8" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
@@ -3136,7 +3139,7 @@
       <c r="E9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>94</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -3154,7 +3157,7 @@
       <c r="K9" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
@@ -3172,7 +3175,7 @@
       <c r="E10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>95</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -3190,7 +3193,7 @@
       <c r="K10" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
@@ -3676,7 +3679,7 @@
       <c r="E24" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="5" t="s">
         <v>89</v>
       </c>
       <c r="G24" s="5" t="s">
@@ -3712,7 +3715,7 @@
       <c r="E25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="5" t="s">
         <v>90</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -3748,7 +3751,7 @@
       <c r="E26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="5" t="s">
         <v>91</v>
       </c>
       <c r="G26" s="5" t="s">
@@ -3784,7 +3787,7 @@
       <c r="E27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G27" s="5" t="s">
@@ -3820,7 +3823,7 @@
       <c r="E28" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="5" t="s">
         <v>93</v>
       </c>
       <c r="G28" s="5" t="s">
@@ -3856,7 +3859,7 @@
       <c r="E29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="5" t="s">
         <v>94</v>
       </c>
       <c r="G29" s="5" t="s">
@@ -3892,7 +3895,7 @@
       <c r="E30" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="5" t="s">
         <v>95</v>
       </c>
       <c r="G30" s="5" t="s">
@@ -4396,7 +4399,7 @@
       <c r="E44" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="5" t="s">
         <v>89</v>
       </c>
       <c r="G44" s="5" t="s">
@@ -4432,7 +4435,7 @@
       <c r="E45" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="5" t="s">
         <v>90</v>
       </c>
       <c r="G45" s="5" t="s">
@@ -4468,7 +4471,7 @@
       <c r="E46" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="5" t="s">
         <v>91</v>
       </c>
       <c r="G46" s="5" t="s">
@@ -4504,7 +4507,7 @@
       <c r="E47" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G47" s="5" t="s">
@@ -4540,7 +4543,7 @@
       <c r="E48" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="5" t="s">
         <v>93</v>
       </c>
       <c r="G48" s="5" t="s">
@@ -4576,7 +4579,7 @@
       <c r="E49" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="5" t="s">
         <v>94</v>
       </c>
       <c r="G49" s="5" t="s">
@@ -4612,7 +4615,7 @@
       <c r="E50" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="5" t="s">
         <v>95</v>
       </c>
       <c r="G50" s="5" t="s">
@@ -5123,13 +5126,13 @@
         <v>63.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L2" s="6"/>
     </row>
@@ -5150,7 +5153,7 @@
         <v>33</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>18</v>
@@ -5159,13 +5162,13 @@
         <v>57.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L3" s="6"/>
     </row>
@@ -5186,7 +5189,7 @@
         <v>33</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>18</v>
@@ -5195,13 +5198,13 @@
         <v>519.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L4" s="6"/>
     </row>
@@ -5222,7 +5225,7 @@
         <v>33</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>18</v>
@@ -5231,13 +5234,13 @@
         <v>940.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L5" s="5"/>
     </row>
@@ -5258,7 +5261,7 @@
         <v>33</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>18</v>
@@ -5267,13 +5270,13 @@
         <v>2700.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L6" s="6"/>
     </row>
@@ -5294,7 +5297,7 @@
         <v>33</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>18</v>
@@ -5303,13 +5306,13 @@
         <v>520.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L7" s="5"/>
     </row>
@@ -5330,7 +5333,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>18</v>
@@ -5339,13 +5342,13 @@
         <v>90.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L8" s="6"/>
     </row>
@@ -5381,7 +5384,7 @@
         <v>50</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L9" s="6"/>
     </row>
@@ -5402,7 +5405,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>106</v>
@@ -5417,7 +5420,7 @@
         <v>50</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L10" s="6"/>
     </row>
@@ -5438,7 +5441,7 @@
         <v>33</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>106</v>
@@ -5453,7 +5456,7 @@
         <v>50</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L11" s="6"/>
     </row>
@@ -5474,7 +5477,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>106</v>
@@ -5489,7 +5492,7 @@
         <v>50</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L12" s="6"/>
     </row>
@@ -5510,7 +5513,7 @@
         <v>33</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>106</v>
@@ -5525,7 +5528,7 @@
         <v>50</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L13" s="6"/>
     </row>
@@ -5546,7 +5549,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>106</v>
@@ -5561,7 +5564,7 @@
         <v>50</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L14" s="6"/>
     </row>
@@ -5582,7 +5585,7 @@
         <v>33</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>106</v>
@@ -5597,7 +5600,7 @@
         <v>50</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L15" s="6"/>
     </row>
@@ -5633,7 +5636,7 @@
         <v>50</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L16" s="6"/>
     </row>
@@ -5654,7 +5657,7 @@
         <v>33</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>108</v>
@@ -5669,7 +5672,7 @@
         <v>50</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L17" s="6"/>
     </row>
@@ -5690,7 +5693,7 @@
         <v>33</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>108</v>
@@ -5705,7 +5708,7 @@
         <v>50</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L18" s="6"/>
     </row>
@@ -5726,7 +5729,7 @@
         <v>33</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>108</v>
@@ -5741,7 +5744,7 @@
         <v>50</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L19" s="6"/>
     </row>
@@ -5762,7 +5765,7 @@
         <v>33</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>108</v>
@@ -5777,7 +5780,7 @@
         <v>50</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L20" s="5"/>
     </row>
@@ -5798,7 +5801,7 @@
         <v>33</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>108</v>
@@ -5813,7 +5816,7 @@
         <v>50</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L21" s="6"/>
     </row>
@@ -5834,7 +5837,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>108</v>
@@ -5849,7 +5852,7 @@
         <v>50</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L22" s="6"/>
     </row>
@@ -5912,7 +5915,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -5924,7 +5927,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -5932,16 +5935,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>14</v>
@@ -5962,36 +5965,36 @@
         <v>19</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>18</v>
@@ -6006,36 +6009,36 @@
         <v>19</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>18</v>
@@ -6050,36 +6053,36 @@
         <v>19</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>18</v>
@@ -6094,36 +6097,36 @@
         <v>19</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>18</v>
@@ -6138,36 +6141,36 @@
         <v>19</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>18</v>
@@ -6182,36 +6185,36 @@
         <v>19</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>18</v>
@@ -6226,36 +6229,36 @@
         <v>19</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>18</v>
@@ -6270,36 +6273,36 @@
         <v>19</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>18</v>
@@ -6314,36 +6317,36 @@
         <v>19</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>18</v>
@@ -6358,36 +6361,36 @@
         <v>19</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>18</v>
@@ -6405,31 +6408,31 @@
         <v>50</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>18</v>
@@ -6447,31 +6450,31 @@
         <v>50</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="N13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>18</v>
@@ -6489,31 +6492,31 @@
         <v>50</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>18</v>
@@ -6531,31 +6534,31 @@
         <v>50</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="N15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>18</v>
@@ -6573,31 +6576,31 @@
         <v>50</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>18</v>
@@ -6615,31 +6618,31 @@
         <v>50</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>18</v>
@@ -6657,31 +6660,31 @@
         <v>50</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>18</v>
@@ -6699,31 +6702,31 @@
         <v>50</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>18</v>
@@ -6741,10 +6744,10 @@
         <v>50</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="N20" s="5"/>
     </row>

</xml_diff>